<commit_message>
Added Form and FFill script
</commit_message>
<xml_diff>
--- a/3D printer projects/3D Printer with accessories.xlsx
+++ b/3D printer projects/3D Printer with accessories.xlsx
@@ -2147,32 +2147,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004A03003CA21BDE4E84D38E456462318A" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bf987b0958463ab045a25897fa7312e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="700a75ce-dd9d-411b-bd1e-ab93f39097ba" xmlns:ns3="ce04ccd7-686d-4e9d-9396-1513c4faabae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f83d4cb975e74129b6b577627f4ba55" ns2:_="" ns3:_="">
-    <xsd:import namespace="700a75ce-dd9d-411b-bd1e-ab93f39097ba"/>
-    <xsd:import namespace="ce04ccd7-686d-4e9d-9396-1513c4faabae"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE4CDFAD8D29F44BA3595B26EBF98D7E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="866addd3bc14dc82dc60b51d940083c6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="3bba17b1-ca09-4865-ba6f-0714c5739852" xmlns:ns4="4decd463-a3dd-4fb0-bb57-735c1a8c741d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e874a30f38c26bb096d99537478574ce" ns1:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="3bba17b1-ca09-4865-ba6f-0714c5739852"/>
+    <xsd:import namespace="4decd463-a3dd-4fb0-bb57-735c1a8c741d"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:Content_x0020_Author_x0020_Email" minOccurs="0"/>
+                <xsd:element ref="ns1:RoutingRuleDescription" minOccurs="0"/>
+                <xsd:element ref="ns3:Content_x0020_Owner1" minOccurs="0"/>
+                <xsd:element ref="ns3:Record" minOccurs="0"/>
+                <xsd:element ref="ns3:Record_x0020_Series_x0020_Number" minOccurs="0"/>
+                <xsd:element ref="ns1:Language" minOccurs="0"/>
+                <xsd:element ref="ns3:Sensitivity" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns3:nd4e770dece24acd81cc5ad0e0f5f382" minOccurs="0"/>
+                <xsd:element ref="ns3:me5168d4f87948a08fcc94d4eeda3704" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns4:Group" minOccurs="0"/>
+                <xsd:element ref="ns4:ProjectName" minOccurs="0"/>
+                <xsd:element ref="ns4:Tags" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2180,88 +2183,75 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="700a75ce-dd9d-411b-bd1e-ab93f39097ba" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="RoutingRuleDescription" ma:index="4" nillable="true" ma:displayName="Description" ma:internalName="RoutingRuleDescription" ma:readOnly="false">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
+        <xsd:restriction base="dms:Text">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="f53c2da0-965e-4c49-9e20-3f7554834061" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="Language" ma:index="9" nillable="true" ma:displayName="Language" ma:default="English" ma:internalName="Language" ma:readOnly="false">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="20" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="21" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
+        <xsd:union memberTypes="dms:Text">
+          <xsd:simpleType>
+            <xsd:restriction base="dms:Choice">
+              <xsd:enumeration value="Arabic (Saudi Arabia)"/>
+              <xsd:enumeration value="Bulgarian (Bulgaria)"/>
+              <xsd:enumeration value="Chinese (Hong Kong S.A.R.)"/>
+              <xsd:enumeration value="Chinese (China)"/>
+              <xsd:enumeration value="Chinese (Taiwan)"/>
+              <xsd:enumeration value="Croatian (Croatia)"/>
+              <xsd:enumeration value="Czech (Czech Republic)"/>
+              <xsd:enumeration value="Danish (Denmark)"/>
+              <xsd:enumeration value="Dutch (Netherlands)"/>
+              <xsd:enumeration value="English"/>
+              <xsd:enumeration value="Estonian (Estonia)"/>
+              <xsd:enumeration value="Finnish (Finland)"/>
+              <xsd:enumeration value="French (France)"/>
+              <xsd:enumeration value="German (Germany)"/>
+              <xsd:enumeration value="Greek (Greece)"/>
+              <xsd:enumeration value="Hebrew (Israel)"/>
+              <xsd:enumeration value="Hindi (India)"/>
+              <xsd:enumeration value="Hungarian (Hungary)"/>
+              <xsd:enumeration value="Indonesian (Indonesia)"/>
+              <xsd:enumeration value="Italian (Italy)"/>
+              <xsd:enumeration value="Japanese (Japan)"/>
+              <xsd:enumeration value="Korean (Korea)"/>
+              <xsd:enumeration value="Latvian (Latvia)"/>
+              <xsd:enumeration value="Lithuanian (Lithuania)"/>
+              <xsd:enumeration value="Malay (Malaysia)"/>
+              <xsd:enumeration value="Norwegian (Bokmal) (Norway)"/>
+              <xsd:enumeration value="Polish (Poland)"/>
+              <xsd:enumeration value="Portuguese (Brazil)"/>
+              <xsd:enumeration value="Portuguese (Portugal)"/>
+              <xsd:enumeration value="Romanian (Romania)"/>
+              <xsd:enumeration value="Russian (Russia)"/>
+              <xsd:enumeration value="Serbian (Latin) (Serbia)"/>
+              <xsd:enumeration value="Slovak (Slovakia)"/>
+              <xsd:enumeration value="Slovenian (Slovenia)"/>
+              <xsd:enumeration value="Spanish (Spain)"/>
+              <xsd:enumeration value="Swedish (Sweden)"/>
+              <xsd:enumeration value="Thai (Thailand)"/>
+              <xsd:enumeration value="Turkish (Turkey)"/>
+              <xsd:enumeration value="Ukrainian (Ukraine)"/>
+              <xsd:enumeration value="Urdu (Islamic Republic of Pakistan)"/>
+              <xsd:enumeration value="Vietnamese (Vietnam)"/>
+            </xsd:restriction>
+          </xsd:simpleType>
+        </xsd:union>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ce04ccd7-686d-4e9d-9396-1513c4faabae" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3bba17b1-ca09-4865-ba6f-0714c5739852" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="Content_x0020_Author_x0020_Email" ma:index="3" nillable="true" ma:displayName="Content Author Email" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Content_x0020_Author_x0020_Email" ma:readOnly="false" ma:showField="ImnName">
       <xsd:complexType>
         <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
+          <xsd:extension base="dms:User">
             <xsd:sequence>
               <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
                 <xsd:complexType>
@@ -2277,14 +2267,71 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="Content_x0020_Owner1" ma:index="6" nillable="true" ma:displayName="Content Owner" ma:description="Identifies the business owner responsible for the accuracy and appropriate use of content items. Is generally hidden from view, but is used by the content management system to notify a responsible person that review or other content lifecycle" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Content_x0020_Owner1" ma:readOnly="false" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Record" ma:index="7" nillable="true" ma:displayName="Record" ma:default="0" ma:description="​For collaborative or normal documents, the default is set to No." ma:internalName="Record" ma:readOnly="false">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Record_x0020_Series_x0020_Number" ma:index="8" nillable="true" ma:displayName="Record Series Number" ma:description="​If the record tag is set to yes, a valid Record Series Number (as defined by RM-00-001.AV is required to be present." ma:internalName="Record_x0020_Series_x0020_Number" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="18" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{1fa85080-ac94-413f-b681-65d02312a39a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="ce04ccd7-686d-4e9d-9396-1513c4faabae">
+    <xsd:element name="Sensitivity" ma:index="10" nillable="true" ma:displayName="Sensitivity" ma:default="Internal" ma:description="​Security level required by the content . Values = Public, Internal, Restricted, Secret" ma:format="Dropdown" ma:internalName="Sensitivity" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Public"/>
+          <xsd:enumeration value="Internal"/>
+          <xsd:enumeration value="Restricted"/>
+          <xsd:enumeration value="Secret"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="12" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{52c9f977-e2e7-4cdf-85bf-9dbca809ee38}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="88998b2f-5cc8-475d-b9b4-a8d353d33050">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="nd4e770dece24acd81cc5ad0e0f5f382" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="nd4e770dece24acd81cc5ad0e0f5f382" ma:taxonomyFieldName="Document_x0020_Categories" ma:displayName="Document Categories" ma:readOnly="false" ma:fieldId="{7d4e770d-ece2-4acd-81cc-5ad0e0f5f382}" ma:sspId="f53c2da0-965e-4c49-9e20-3f7554834061" ma:termSetId="0bc447bc-cd5f-4a5b-8cef-40c06dd94379" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="me5168d4f87948a08fcc94d4eeda3704" ma:index="15" nillable="true" ma:displayName="Topic Column_0" ma:hidden="true" ma:internalName="me5168d4f87948a08fcc94d4eeda3704" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{52c9f977-e2e7-4cdf-85bf-9dbca809ee38}" ma:internalName="TaxCatchAll" ma:readOnly="false" ma:showField="CatchAllData" ma:web="88998b2f-5cc8-475d-b9b4-a8d353d33050">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -2296,17 +2343,73 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4decd463-a3dd-4fb0-bb57-735c1a8c741d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="22" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="23" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="24" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="25" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Group" ma:index="26" nillable="true" ma:displayName="Group" ma:format="Dropdown" ma:internalName="Group">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="CCD"/>
+          <xsd:enumeration value="Pilot Lab"/>
+          <xsd:enumeration value="Purification Development"/>
+          <xsd:enumeration value="S&amp;T"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ProjectName" ma:index="27" nillable="true" ma:displayName="Project Name" ma:format="Dropdown" ma:internalName="ProjectName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Tags" ma:index="28" nillable="true" ma:displayName="Tags" ma:format="Dropdown" ma:internalName="Tags">
+      <xsd:simpleType>
+        <xsd:union memberTypes="dms:Text">
+          <xsd:simpleType>
+            <xsd:restriction base="dms:Choice">
+              <xsd:enumeration value="Quote"/>
+              <xsd:enumeration value="Presentation"/>
+              <xsd:enumeration value="script"/>
+              <xsd:enumeration value="reference"/>
+              <xsd:enumeration value="template"/>
+            </xsd:restriction>
+          </xsd:simpleType>
+        </xsd:union>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
     <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
     <xsd:element name="coreProperties" type="CT_coreProperties"/>
     <xsd:complexType name="CT_coreProperties">
       <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1" ma:index="2" ma:displayName="Author"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="16" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2398,10 +2501,33 @@
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="700a75ce-dd9d-411b-bd1e-ab93f39097ba">
+    <TaxCatchAll xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <ProjectName xmlns="4decd463-a3dd-4fb0-bb57-735c1a8c741d" xsi:nil="true"/>
+    <Group xmlns="4decd463-a3dd-4fb0-bb57-735c1a8c741d" xsi:nil="true"/>
+    <Content_x0020_Author_x0020_Email xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Content_x0020_Author_x0020_Email>
+    <Record_x0020_Series_x0020_Number xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852" xsi:nil="true"/>
+    <me5168d4f87948a08fcc94d4eeda3704 xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852" xsi:nil="true"/>
+    <Content_x0020_Owner1 xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Content_x0020_Owner1>
+    <nd4e770dece24acd81cc5ad0e0f5f382 xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ce04ccd7-686d-4e9d-9396-1513c4faabae" xsi:nil="true"/>
+    </nd4e770dece24acd81cc5ad0e0f5f382>
+    <RoutingRuleDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Sensitivity xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852">Internal</Sensitivity>
+    <Tags xmlns="4decd463-a3dd-4fb0-bb57-735c1a8c741d" xsi:nil="true"/>
+    <Record xmlns="3bba17b1-ca09-4865-ba6f-0714c5739852">false</Record>
   </documentManagement>
 </p:properties>
 </file>
@@ -2415,23 +2541,13 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f53c2da0-965e-4c49-9e20-3f7554834061" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401017F7-F9EC-4D45-B878-285544981B23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="700a75ce-dd9d-411b-bd1e-ab93f39097ba"/>
-    <ds:schemaRef ds:uri="ce04ccd7-686d-4e9d-9396-1513c4faabae"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6934318-5DD3-44F6-888E-89963154C11E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2451,4 +2567,8 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444067A3-5099-4DC4-8B7D-7130ADEA8115}"/>
 </file>
</xml_diff>